<commit_message>
Fixed a bug with the stencils list.   must call force close function to clear this variable.  Can't set to null Also added line pattern resulotion in the Excel Data file supports Solid, Dashed, Dotted and Dash_Dot Update to the user guide
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_BlueprintingDataFile_Template.xlsx
+++ b/Data/ScriptData/OC_BlueprintingDataFile_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9FD178C-BB5F-4190-BD16-5CA98344C7F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79C105A-0E1F-489E-956F-617479633DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18840" yWindow="300" windowWidth="27375" windowHeight="15330" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
+    <workbookView xWindow="-27330" yWindow="345" windowWidth="27375" windowHeight="15330" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -235,7 +235,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="119">
   <si>
     <t>mach_name</t>
   </si>
@@ -553,6 +553,55 @@
   </si>
   <si>
     <t>To Line Color</t>
+  </si>
+  <si>
+    <t>Line Pattern</t>
+  </si>
+  <si>
+    <t>Solid</t>
+  </si>
+  <si>
+    <t>Dashed</t>
+  </si>
+  <si>
+    <t>Dotted</t>
+  </si>
+  <si>
+    <t>Dash_Dot</t>
+  </si>
+  <si>
+    <t>;Test Shapes</t>
+  </si>
+  <si>
+    <t>Server:OC-T1</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OmniCenter Test Server
+Cloud Hosted
+</t>
+  </si>
+  <si>
+    <t>xxx.xxx.xxx.xxx</t>
+  </si>
+  <si>
+    <t>Server:OSI-T1</t>
+  </si>
+  <si>
+    <t>OIS Test Server
+Cloud Hosted</t>
+  </si>
+  <si>
+    <t>OISInterfaces:T1</t>
+  </si>
+  <si>
+    <t>OISInterfaces</t>
+  </si>
+  <si>
+    <t>OIS Test
+Interfaces</t>
   </si>
 </sst>
 </file>
@@ -721,7 +770,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -822,6 +871,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1158,11 +1210,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6B3580-88F6-4152-BCD8-7BDA3AA42961}">
-  <dimension ref="A1:AF14"/>
+  <dimension ref="A1:AF18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB1" sqref="AB1"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AD13" sqref="AD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,7 +1222,7 @@
     <col min="1" max="1" width="23.7109375" style="25" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="37.85546875" style="24" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="17" max="17" width="8" customWidth="1"/>
@@ -1180,6 +1232,7 @@
     <col min="25" max="25" width="14.42578125" customWidth="1"/>
     <col min="26" max="26" width="13.28515625" customWidth="1"/>
     <col min="27" max="27" width="10.28515625" customWidth="1"/>
+    <col min="28" max="28" width="16.5703125" customWidth="1"/>
     <col min="29" max="29" width="11" customWidth="1"/>
     <col min="30" max="30" width="12" customWidth="1"/>
     <col min="32" max="32" width="11.7109375" customWidth="1"/>
@@ -1360,21 +1413,13 @@
       <c r="V3" s="10"/>
       <c r="W3" s="8"/>
       <c r="X3" s="7"/>
-      <c r="Y3" s="11">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
       <c r="AA3" s="7"/>
       <c r="AB3" s="7"/>
       <c r="AC3" s="7"/>
-      <c r="AD3" s="11">
-        <v>1</v>
-      </c>
-      <c r="AE3" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="11"/>
       <c r="AF3" s="7"/>
     </row>
     <row r="4" spans="1:32" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1416,21 +1461,13 @@
       <c r="V4" s="10"/>
       <c r="W4" s="8"/>
       <c r="X4" s="7"/>
-      <c r="Y4" s="11">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
       <c r="AA4" s="7"/>
       <c r="AB4" s="7"/>
       <c r="AC4" s="7"/>
-      <c r="AD4" s="11">
-        <v>1</v>
-      </c>
-      <c r="AE4" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="AD4" s="11"/>
+      <c r="AE4" s="11"/>
       <c r="AF4" s="7"/>
     </row>
     <row r="5" spans="1:32" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1474,26 +1511,18 @@
       <c r="V5" s="10"/>
       <c r="W5" s="8"/>
       <c r="X5" s="7"/>
-      <c r="Y5" s="11">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="Y5" s="11"/>
+      <c r="Z5" s="11"/>
       <c r="AA5" s="7"/>
       <c r="AB5" s="7"/>
       <c r="AC5" s="7"/>
-      <c r="AD5" s="11">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="AD5" s="11"/>
+      <c r="AE5" s="11"/>
       <c r="AF5" s="7"/>
     </row>
     <row r="6" spans="1:32" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="35">
-        <v>0</v>
+      <c r="A6" s="35" t="s">
+        <v>85</v>
       </c>
       <c r="B6" s="36" t="s">
         <v>86</v>
@@ -1532,21 +1561,13 @@
       <c r="V6" s="10"/>
       <c r="W6" s="8"/>
       <c r="X6" s="7"/>
-      <c r="Y6" s="11">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
       <c r="AA6" s="7"/>
       <c r="AB6" s="7"/>
       <c r="AC6" s="7"/>
-      <c r="AD6" s="11">
-        <v>1</v>
-      </c>
-      <c r="AE6" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
       <c r="AF6" s="7"/>
     </row>
     <row r="7" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1626,21 +1647,13 @@
       <c r="V8" s="10"/>
       <c r="W8" s="8"/>
       <c r="X8" s="7"/>
-      <c r="Y8" s="11">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
       <c r="AA8" s="7"/>
       <c r="AB8" s="7"/>
       <c r="AC8" s="7"/>
-      <c r="AD8" s="11">
-        <v>1</v>
-      </c>
-      <c r="AE8" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="11"/>
       <c r="AF8" s="7"/>
     </row>
     <row r="9" spans="1:32" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1686,21 +1699,13 @@
       <c r="V9" s="10"/>
       <c r="W9" s="8"/>
       <c r="X9" s="7"/>
-      <c r="Y9" s="11">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="Y9" s="11"/>
+      <c r="Z9" s="11"/>
       <c r="AA9" s="7"/>
       <c r="AB9" s="7"/>
       <c r="AC9" s="7"/>
-      <c r="AD9" s="11">
-        <v>1</v>
-      </c>
-      <c r="AE9" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="AD9" s="11"/>
+      <c r="AE9" s="11"/>
       <c r="AF9" s="7"/>
     </row>
     <row r="10" spans="1:32" s="12" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1748,26 +1753,18 @@
       <c r="V10" s="10"/>
       <c r="W10" s="8"/>
       <c r="X10" s="7"/>
-      <c r="Y10" s="11">
-        <v>1</v>
-      </c>
-      <c r="Z10" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
       <c r="AA10" s="7"/>
       <c r="AB10" s="7"/>
       <c r="AC10" s="7"/>
-      <c r="AD10" s="11">
-        <v>1</v>
-      </c>
-      <c r="AE10" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
       <c r="AF10" s="7"/>
     </row>
-    <row r="11" spans="1:32" s="6" customFormat="1" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
@@ -1801,20 +1798,22 @@
       <c r="AE11" s="16"/>
       <c r="AF11" s="16"/>
     </row>
-    <row r="12" spans="1:32" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>2</v>
+    <row r="12" spans="1:32" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>1</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="22"/>
+        <v>111</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>112</v>
+      </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -1824,14 +1823,16 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
-      <c r="O12" s="9"/>
+      <c r="O12" s="9" t="s">
+        <v>113</v>
+      </c>
       <c r="P12" s="9"/>
       <c r="Q12" s="7"/>
       <c r="R12" s="10">
-        <v>0.25</v>
+        <v>4.875</v>
       </c>
       <c r="S12" s="10">
-        <v>10.75</v>
+        <v>6.25</v>
       </c>
       <c r="T12" s="10">
         <v>0</v>
@@ -1839,41 +1840,41 @@
       <c r="U12" s="10">
         <v>0</v>
       </c>
-      <c r="V12" s="10"/>
+      <c r="V12" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="W12" s="8"/>
       <c r="X12" s="7"/>
-      <c r="Y12" s="11">
-        <v>1</v>
-      </c>
-      <c r="Z12" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="Y12" s="11"/>
+      <c r="Z12" s="11"/>
       <c r="AA12" s="7"/>
-      <c r="AB12" s="7"/>
+      <c r="AB12" s="8" t="s">
+        <v>114</v>
+      </c>
       <c r="AC12" s="7"/>
-      <c r="AD12" s="11">
-        <v>1</v>
+      <c r="AD12" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="AE12" s="11" t="s">
         <v>17</v>
       </c>
       <c r="AF12" s="7"/>
     </row>
-    <row r="13" spans="1:32" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
-        <v>2</v>
+    <row r="13" spans="1:32" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>1</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>46</v>
+        <v>114</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>34</v>
+        <v>111</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>115</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -1884,14 +1885,16 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
-      <c r="O13" s="9"/>
+      <c r="O13" s="9" t="s">
+        <v>113</v>
+      </c>
       <c r="P13" s="9"/>
       <c r="Q13" s="7"/>
       <c r="R13" s="10">
-        <v>3.125</v>
+        <v>6.125</v>
       </c>
       <c r="S13" s="10">
-        <v>10.75</v>
+        <v>5.7969999999999997</v>
       </c>
       <c r="T13" s="10">
         <v>0</v>
@@ -1899,45 +1902,45 @@
       <c r="U13" s="10">
         <v>0</v>
       </c>
-      <c r="V13" s="10"/>
+      <c r="V13" s="10" t="s">
+        <v>24</v>
+      </c>
       <c r="W13" s="8"/>
       <c r="X13" s="7"/>
-      <c r="Y13" s="11">
+      <c r="Y13" s="11"/>
+      <c r="Z13" s="11"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF13" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>1</v>
-      </c>
-      <c r="Z13" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA13" s="7"/>
-      <c r="AB13" s="7"/>
-      <c r="AC13" s="7"/>
-      <c r="AD13" s="11">
-        <v>1</v>
-      </c>
-      <c r="AE13" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="AF13" s="7"/>
-    </row>
-    <row r="14" spans="1:32" s="12" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>2</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>47</v>
+        <v>116</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="8">
-        <v>10</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
@@ -1946,40 +1949,228 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="S14" s="9">
-        <v>1.75</v>
-      </c>
-      <c r="T14" s="9">
-        <v>0</v>
-      </c>
-      <c r="U14" s="9">
-        <v>1.125</v>
+      <c r="O14" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="P14" s="9">
+        <v>5001</v>
+      </c>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="10">
+        <v>7.5</v>
+      </c>
+      <c r="S14" s="10">
+        <v>6.0750000000000002</v>
+      </c>
+      <c r="T14" s="10">
+        <v>0</v>
+      </c>
+      <c r="U14" s="10">
+        <v>0</v>
       </c>
       <c r="V14" s="10"/>
       <c r="W14" s="8"/>
       <c r="X14" s="7"/>
-      <c r="Y14" s="11">
-        <v>1</v>
-      </c>
-      <c r="Z14" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
       <c r="AA14" s="7"/>
       <c r="AB14" s="7"/>
       <c r="AC14" s="7"/>
-      <c r="AD14" s="11">
-        <v>1</v>
-      </c>
-      <c r="AE14" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="11"/>
       <c r="AF14" s="7"/>
+    </row>
+    <row r="15" spans="1:32" s="6" customFormat="1" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="16"/>
+      <c r="Z15" s="16"/>
+      <c r="AA15" s="16"/>
+      <c r="AB15" s="16"/>
+      <c r="AC15" s="16"/>
+      <c r="AD15" s="16"/>
+      <c r="AE15" s="16"/>
+      <c r="AF15" s="16"/>
+    </row>
+    <row r="16" spans="1:32" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>2</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="22"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="S16" s="10">
+        <v>10.75</v>
+      </c>
+      <c r="T16" s="10">
+        <v>0</v>
+      </c>
+      <c r="U16" s="10">
+        <v>0</v>
+      </c>
+      <c r="V16" s="10"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="11"/>
+      <c r="Z16" s="11"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="7"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="11"/>
+      <c r="AE16" s="11"/>
+      <c r="AF16" s="7"/>
+    </row>
+    <row r="17" spans="1:32" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>2</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="10">
+        <v>3.125</v>
+      </c>
+      <c r="S17" s="10">
+        <v>10.75</v>
+      </c>
+      <c r="T17" s="10">
+        <v>0</v>
+      </c>
+      <c r="U17" s="10">
+        <v>0</v>
+      </c>
+      <c r="V17" s="10"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="11"/>
+      <c r="Z17" s="11"/>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="11"/>
+      <c r="AE17" s="11"/>
+      <c r="AF17" s="7"/>
+    </row>
+    <row r="18" spans="1:32" s="12" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>2</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="8">
+        <v>10</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="S18" s="9">
+        <v>1.75</v>
+      </c>
+      <c r="T18" s="9">
+        <v>0</v>
+      </c>
+      <c r="U18" s="9">
+        <v>1.125</v>
+      </c>
+      <c r="V18" s="10"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="11"/>
+      <c r="AF18" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1987,24 +2178,30 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E028F679-E2E7-4B73-A1F3-5F8969AC7B09}">
-          <x14:formula1>
-            <xm:f>Tables!$C$2:$C$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>Z8:Z10 AE8:AE10 Z12:Z14 AE12:AE14</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{1B1731AA-F2EB-4AE2-A6BB-599908765112}">
           <x14:formula1>
             <xm:f>Tables!$E$2:$E$16</xm:f>
           </x14:formula1>
-          <xm:sqref>F8:F14</xm:sqref>
+          <xm:sqref>F8:F11 F15:F18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{E07EFBB9-D469-4A17-B52C-CFA259DBA49F}">
           <x14:formula1>
             <xm:f>Tables!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>V8:V14 AA8:AA14 AF8:AF14</xm:sqref>
+          <xm:sqref>AA2:AA18 AF2:AF18 W2:W11 W15:W18 V2:V18</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{03EA1083-D949-46E8-A92C-28C1E75A14F4}">
+          <x14:formula1>
+            <xm:f>Tables!$G$2:$G$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>Y2:Y18 AD2:AD18</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{296B0321-4EB3-4DBF-B3C7-556564F8D22F}">
+          <x14:formula1>
+            <xm:f>Tables!$C$2:$C$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>AE2:AE18 Z2:Z18</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2028,12 +2225,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="32"/>
       <c r="F1" s="32"/>
       <c r="G1" s="31"/>
@@ -2054,12 +2251,12 @@
       <c r="D2" s="26"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
@@ -2100,19 +2297,19 @@
       <c r="D8" s="13"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
@@ -2198,55 +2395,55 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="43"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="44"/>
       <c r="K15" s="28">
         <f>SUM(K12:K14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="48" t="s">
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="I16" s="48"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="50"/>
       <c r="K16" s="29">
         <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="43"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="44"/>
       <c r="K17" s="27">
         <f>SUM(K15:K16)</f>
         <v>150</v>
@@ -2282,10 +2479,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="51"/>
+      <c r="B1" s="52"/>
       <c r="C1" s="30"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2334,19 +2531,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7C7130-C7ED-4E34-8ED2-CC717737ADA7}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="6" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>81</v>
       </c>
@@ -2356,13 +2554,17 @@
       <c r="E1" s="36" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="39" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
       <c r="C2" s="11"/>
       <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>23</v>
       </c>
@@ -2372,8 +2574,11 @@
       <c r="E3" s="11">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>25</v>
       </c>
@@ -2383,8 +2588,11 @@
       <c r="E4" s="11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>28</v>
       </c>
@@ -2394,8 +2602,11 @@
       <c r="E5" s="11">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G5" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>57</v>
       </c>
@@ -2405,8 +2616,11 @@
       <c r="E6" s="11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G6" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>27</v>
       </c>
@@ -2414,7 +2628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>30</v>
       </c>
@@ -2422,7 +2636,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>82</v>
       </c>
@@ -2430,7 +2644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>24</v>
       </c>
@@ -2438,7 +2652,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>32</v>
       </c>
@@ -2446,7 +2660,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>33</v>
       </c>
@@ -2454,30 +2668,30 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="33"/>
       <c r="E13" s="11">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E14" s="11" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E15" s="11">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16" s="34" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:XFD2" xr:uid="{C5F5580C-CDE8-4810-9011-46F88A3A0968}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:F2 O2:XFD2" xr:uid="{C5F5580C-CDE8-4810-9011-46F88A3A0968}">
       <formula1>$A$4:$A$10</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Sorted the User Guide Stencil table
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_BlueprintingDataFile_Template.xlsx
+++ b/Data/ScriptData/OC_BlueprintingDataFile_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Blueprinting_Tool\Data\ScriptData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB407C49-5A72-4EB6-93D2-CAA44FBF5683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DAB4AB-5E1D-4F1B-B7B9-E562B4BC16C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27330" yWindow="345" windowWidth="27375" windowHeight="15330" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
+    <workbookView xWindow="-27975" yWindow="540" windowWidth="27375" windowHeight="15330" activeTab="2" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -641,7 +641,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -693,6 +693,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -770,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -895,6 +901,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1212,9 +1227,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6B3580-88F6-4152-BCD8-7BDA3AA42961}">
   <dimension ref="A1:AF18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD13" sqref="AD13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,16 +1254,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" s="20" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="54" t="s">
         <v>43</v>
       </c>
       <c r="E1" s="21" t="s">
@@ -1290,10 +1305,10 @@
       <c r="Q1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="55" t="s">
         <v>11</v>
       </c>
       <c r="T1" s="3" t="s">
@@ -2469,7 +2484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2329B1A3-4876-444E-9008-3CE76AAF27BE}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -2535,8 +2550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7C7130-C7ED-4E34-8ED2-CC717737ADA7}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed an issue loading a Template with shapes and adding additional stencil file
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_BlueprintingDataFile_Template.xlsx
+++ b/Data/ScriptData/OC_BlueprintingDataFile_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Blueprinting_Tool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D7628C-5AEE-471D-875D-0A257D330CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BFF9A0-DF70-4695-8F60-A4EAA4C137D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9495" yWindow="1755" windowWidth="26505" windowHeight="15330" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
+    <workbookView xWindow="20310" yWindow="1635" windowWidth="26505" windowHeight="15330" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -235,7 +235,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="155">
   <si>
     <t>mach_name</t>
   </si>
@@ -487,19 +487,10 @@
     <t>Using a Visio Template that contains a custom Stencil</t>
   </si>
   <si>
-    <t>Custom Stencil for OmniCell Architech Visio Diagram</t>
-  </si>
-  <si>
     <t>Custom Stencil</t>
   </si>
   <si>
     <t>C:\Omnicell_Blueprinting_Tool\Data\Templates\OC_BlueprintingTemplate.vstx</t>
-  </si>
-  <si>
-    <t>C:\Omnicell_Blueprinting_Tool\Data\Stencils\OC_BlueprintingStencils.vssx</t>
-  </si>
-  <si>
-    <t>C:\Omnicell_Blueprinting_Tool\Data\Stencils\Advocate_CustomStencils.vssx</t>
   </si>
   <si>
     <t>Shape Label Font Size</t>
@@ -632,16 +623,10 @@
     <t>Group2</t>
   </si>
   <si>
-    <t>GroupBD</t>
-  </si>
-  <si>
     <t>IconKey</t>
   </si>
   <si>
     <t>IconKey2</t>
-  </si>
-  <si>
-    <t>IconKeyDash</t>
   </si>
   <si>
     <t>IVX</t>
@@ -706,6 +691,24 @@
   </si>
   <si>
     <t>;comment</t>
+  </si>
+  <si>
+    <t>Group3</t>
+  </si>
+  <si>
+    <t>DashOutline</t>
+  </si>
+  <si>
+    <t>Server2</t>
+  </si>
+  <si>
+    <t>Server3</t>
+  </si>
+  <si>
+    <t>Group4</t>
+  </si>
+  <si>
+    <t>C:\Omnicell_Blueprinting_Tool\Data\Stencils\Account_CustomStencils.vssx</t>
   </si>
 </sst>
 </file>
@@ -1001,6 +1004,12 @@
     <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1021,12 +1030,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1343,11 +1346,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6B3580-88F6-4152-BCD8-7BDA3AA42961}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AF17"/>
+  <dimension ref="A1:AF16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1388,7 +1391,7 @@
         <v>41</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
@@ -1442,31 +1445,31 @@
         <v>33</v>
       </c>
       <c r="X1" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y1" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="Z1" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA1" s="18" t="s">
         <v>88</v>
-      </c>
-      <c r="Y1" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z1" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="AA1" s="18" t="s">
-        <v>91</v>
       </c>
       <c r="AB1" s="5" t="s">
         <v>36</v>
       </c>
       <c r="AC1" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="AD1" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE1" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF1" s="19" t="s">
         <v>92</v>
-      </c>
-      <c r="AD1" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="AE1" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="AF1" s="19" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1506,14 +1509,14 @@
       <c r="AF2" s="16"/>
     </row>
     <row r="3" spans="1:32" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
-        <v>78</v>
+      <c r="A3" s="37">
+        <v>0</v>
       </c>
       <c r="B3" s="38" t="s">
         <v>77</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8" t="s">
@@ -1556,14 +1559,14 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="4" spans="1:32" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="37">
-        <v>0</v>
+      <c r="A4" s="37" t="s">
+        <v>78</v>
       </c>
       <c r="B4" s="38" t="s">
         <v>79</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>85</v>
+        <v>154</v>
       </c>
       <c r="D4" s="38"/>
       <c r="E4" s="38" t="s">
@@ -1605,93 +1608,93 @@
       <c r="AE4" s="11"/>
       <c r="AF4" s="7"/>
     </row>
-    <row r="5" spans="1:32" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="37">
+    <row r="5" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="17"/>
+      <c r="U5" s="17"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="16"/>
+      <c r="AA5" s="16"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="16"/>
+      <c r="AD5" s="16"/>
+      <c r="AE5" s="16"/>
+      <c r="AF5" s="16"/>
+    </row>
+    <row r="6" spans="1:32" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>1</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="S6" s="10">
+        <v>10.75</v>
+      </c>
+      <c r="T6" s="10">
         <v>0</v>
       </c>
-      <c r="B5" s="38" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="10">
+      <c r="U6" s="10">
         <v>0</v>
       </c>
-      <c r="S5" s="10">
-        <v>0</v>
-      </c>
-      <c r="T5" s="10">
-        <v>0</v>
-      </c>
-      <c r="U5" s="10">
-        <v>0</v>
-      </c>
-      <c r="V5" s="10"/>
-      <c r="W5" s="8"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="11"/>
-      <c r="AE5" s="11"/>
-      <c r="AF5" s="7"/>
-    </row>
-    <row r="6" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="17"/>
-      <c r="W6" s="14"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="16"/>
-      <c r="AA6" s="16"/>
-      <c r="AB6" s="16"/>
-      <c r="AC6" s="16"/>
-      <c r="AD6" s="16"/>
-      <c r="AE6" s="16"/>
-      <c r="AF6" s="16"/>
-    </row>
-    <row r="7" spans="1:32" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V6" s="10"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="7"/>
+    </row>
+    <row r="7" spans="1:32" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>1</v>
       </c>
@@ -1699,12 +1702,14 @@
         <v>14</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="22"/>
+        <v>17</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -1718,7 +1723,7 @@
       <c r="P7" s="9"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="10">
-        <v>0.25</v>
+        <v>3.125</v>
       </c>
       <c r="S7" s="10">
         <v>10.75</v>
@@ -1741,7 +1746,7 @@
       <c r="AE7" s="11"/>
       <c r="AF7" s="7"/>
     </row>
-    <row r="8" spans="1:32" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" s="12" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>1</v>
       </c>
@@ -1749,15 +1754,17 @@
         <v>14</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="8"/>
+        <v>32</v>
+      </c>
+      <c r="F8" s="8">
+        <v>10</v>
+      </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
@@ -1768,18 +1775,18 @@
       <c r="N8" s="8"/>
       <c r="O8" s="9"/>
       <c r="P8" s="9"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="10">
-        <v>3.125</v>
-      </c>
-      <c r="S8" s="10">
-        <v>10.75</v>
-      </c>
-      <c r="T8" s="10">
+      <c r="Q8" s="8"/>
+      <c r="R8" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="S8" s="9">
+        <v>1.75</v>
+      </c>
+      <c r="T8" s="9">
         <v>0</v>
       </c>
-      <c r="U8" s="10">
-        <v>0</v>
+      <c r="U8" s="9">
+        <v>1.125</v>
       </c>
       <c r="V8" s="10"/>
       <c r="W8" s="8"/>
@@ -1793,97 +1800,107 @@
       <c r="AE8" s="11"/>
       <c r="AF8" s="7"/>
     </row>
-    <row r="9" spans="1:32" s="12" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+    <row r="9" spans="1:32" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="16"/>
+      <c r="Y9" s="16"/>
+      <c r="Z9" s="16"/>
+      <c r="AA9" s="16"/>
+      <c r="AB9" s="16"/>
+      <c r="AC9" s="16"/>
+      <c r="AD9" s="16"/>
+      <c r="AE9" s="16"/>
+      <c r="AF9" s="16"/>
+    </row>
+    <row r="10" spans="1:32" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>1</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="8">
-        <v>10</v>
-      </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="S9" s="9">
-        <v>1.75</v>
-      </c>
-      <c r="T9" s="9">
+      <c r="C10" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="10">
+        <v>4.875</v>
+      </c>
+      <c r="S10" s="10">
+        <v>6.25</v>
+      </c>
+      <c r="T10" s="10">
         <v>0</v>
       </c>
-      <c r="U9" s="9">
-        <v>1.125</v>
-      </c>
-      <c r="V9" s="10"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="7"/>
-      <c r="AB9" s="7"/>
-      <c r="AC9" s="7"/>
-      <c r="AD9" s="11"/>
-      <c r="AE9" s="11"/>
-      <c r="AF9" s="7"/>
-    </row>
-    <row r="10" spans="1:32" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="17"/>
-      <c r="V10" s="17"/>
-      <c r="W10" s="14"/>
-      <c r="X10" s="16"/>
-      <c r="Y10" s="16"/>
-      <c r="Z10" s="16"/>
-      <c r="AA10" s="16"/>
-      <c r="AB10" s="16"/>
-      <c r="AC10" s="16"/>
-      <c r="AD10" s="16"/>
-      <c r="AE10" s="16"/>
-      <c r="AF10" s="16"/>
-    </row>
-    <row r="11" spans="1:32" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="U10" s="10">
+        <v>0</v>
+      </c>
+      <c r="V10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="W10" s="8"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF10" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>1</v>
       </c>
@@ -1891,10 +1908,10 @@
         <v>14</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>103</v>
@@ -1909,15 +1926,15 @@
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
       <c r="O11" s="9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="P11" s="9"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="10">
-        <v>4.875</v>
+        <v>6.125</v>
       </c>
       <c r="S11" s="10">
-        <v>6.25</v>
+        <v>5.7969999999999997</v>
       </c>
       <c r="T11" s="10">
         <v>0</v>
@@ -1934,14 +1951,14 @@
       <c r="Z11" s="11"/>
       <c r="AA11" s="7"/>
       <c r="AB11" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AC11" s="7"/>
       <c r="AD11" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AE11" s="11" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="AF11" s="7" t="s">
         <v>20</v>
@@ -1955,10 +1972,10 @@
         <v>14</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>106</v>
@@ -1973,15 +1990,17 @@
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
       <c r="O12" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="P12" s="9"/>
+        <v>101</v>
+      </c>
+      <c r="P12" s="9">
+        <v>5001</v>
+      </c>
       <c r="Q12" s="7"/>
       <c r="R12" s="10">
-        <v>6.125</v>
+        <v>7.5</v>
       </c>
       <c r="S12" s="10">
-        <v>5.7969999999999997</v>
+        <v>6.0750000000000002</v>
       </c>
       <c r="T12" s="10">
         <v>0</v>
@@ -1989,123 +2008,107 @@
       <c r="U12" s="10">
         <v>0</v>
       </c>
-      <c r="V12" s="10" t="s">
-        <v>21</v>
-      </c>
+      <c r="V12" s="10"/>
       <c r="W12" s="8"/>
       <c r="X12" s="7"/>
       <c r="Y12" s="11"/>
       <c r="Z12" s="11"/>
       <c r="AA12" s="7"/>
-      <c r="AB12" s="8" t="s">
-        <v>107</v>
-      </c>
+      <c r="AB12" s="7"/>
       <c r="AC12" s="7"/>
-      <c r="AD12" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="AE12" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF12" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>1</v>
-      </c>
-      <c r="B13" s="8" t="s">
+      <c r="AD12" s="11"/>
+      <c r="AE12" s="11"/>
+      <c r="AF12" s="7"/>
+    </row>
+    <row r="13" spans="1:32" s="6" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="14"/>
+      <c r="X13" s="16"/>
+      <c r="Y13" s="16"/>
+      <c r="Z13" s="16"/>
+      <c r="AA13" s="16"/>
+      <c r="AB13" s="16"/>
+      <c r="AC13" s="16"/>
+      <c r="AD13" s="16"/>
+      <c r="AE13" s="16"/>
+      <c r="AF13" s="16"/>
+    </row>
+    <row r="14" spans="1:32" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>2</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="P13" s="9">
-        <v>5001</v>
-      </c>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="10">
-        <v>7.5</v>
-      </c>
-      <c r="S13" s="10">
-        <v>6.0750000000000002</v>
-      </c>
-      <c r="T13" s="10">
+      <c r="C14" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="22"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="S14" s="10">
+        <v>10.75</v>
+      </c>
+      <c r="T14" s="10">
         <v>0</v>
       </c>
-      <c r="U13" s="10">
+      <c r="U14" s="10">
         <v>0</v>
       </c>
-      <c r="V13" s="10"/>
-      <c r="W13" s="8"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11"/>
-      <c r="AA13" s="7"/>
-      <c r="AB13" s="7"/>
-      <c r="AC13" s="7"/>
-      <c r="AD13" s="11"/>
-      <c r="AE13" s="11"/>
-      <c r="AF13" s="7"/>
-    </row>
-    <row r="14" spans="1:32" s="6" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="17"/>
-      <c r="U14" s="17"/>
-      <c r="V14" s="17"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="16"/>
-      <c r="Y14" s="16"/>
-      <c r="Z14" s="16"/>
-      <c r="AA14" s="16"/>
-      <c r="AB14" s="16"/>
-      <c r="AC14" s="16"/>
-      <c r="AD14" s="16"/>
-      <c r="AE14" s="16"/>
-      <c r="AF14" s="16"/>
-    </row>
-    <row r="15" spans="1:32" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V14" s="10"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="11"/>
+      <c r="AF14" s="7"/>
+    </row>
+    <row r="15" spans="1:32" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>2</v>
       </c>
@@ -2113,12 +2116,14 @@
         <v>14</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="22"/>
+        <v>17</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>31</v>
+      </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -2132,7 +2137,7 @@
       <c r="P15" s="9"/>
       <c r="Q15" s="7"/>
       <c r="R15" s="10">
-        <v>0.25</v>
+        <v>3.125</v>
       </c>
       <c r="S15" s="10">
         <v>10.75</v>
@@ -2155,7 +2160,7 @@
       <c r="AE15" s="11"/>
       <c r="AF15" s="7"/>
     </row>
-    <row r="16" spans="1:32" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" s="12" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>2</v>
       </c>
@@ -2163,15 +2168,17 @@
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="8"/>
+        <v>32</v>
+      </c>
+      <c r="F16" s="8">
+        <v>10</v>
+      </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
@@ -2182,18 +2189,18 @@
       <c r="N16" s="8"/>
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="10">
-        <v>3.125</v>
-      </c>
-      <c r="S16" s="10">
-        <v>10.75</v>
-      </c>
-      <c r="T16" s="10">
+      <c r="Q16" s="8"/>
+      <c r="R16" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="S16" s="9">
+        <v>1.75</v>
+      </c>
+      <c r="T16" s="9">
         <v>0</v>
       </c>
-      <c r="U16" s="10">
-        <v>0</v>
+      <c r="U16" s="9">
+        <v>1.125</v>
       </c>
       <c r="V16" s="10"/>
       <c r="W16" s="8"/>
@@ -2207,60 +2214,6 @@
       <c r="AE16" s="11"/>
       <c r="AF16" s="7"/>
     </row>
-    <row r="17" spans="1:32" s="12" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>2</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="8">
-        <v>10</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="S17" s="9">
-        <v>1.75</v>
-      </c>
-      <c r="T17" s="9">
-        <v>0</v>
-      </c>
-      <c r="U17" s="9">
-        <v>1.125</v>
-      </c>
-      <c r="V17" s="10"/>
-      <c r="W17" s="8"/>
-      <c r="X17" s="7"/>
-      <c r="Y17" s="11"/>
-      <c r="Z17" s="11"/>
-      <c r="AA17" s="7"/>
-      <c r="AB17" s="7"/>
-      <c r="AC17" s="7"/>
-      <c r="AD17" s="11"/>
-      <c r="AE17" s="11"/>
-      <c r="AF17" s="7"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2272,31 +2225,31 @@
           <x14:formula1>
             <xm:f>Tables!$E$2:$E$16</xm:f>
           </x14:formula1>
-          <xm:sqref>F7:F10 F14:F17</xm:sqref>
+          <xm:sqref>F6:F9 F13:F16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{E07EFBB9-D469-4A17-B52C-CFA259DBA49F}">
           <x14:formula1>
             <xm:f>Tables!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>W14:W17 V2:V17 W2:W10 AF2:AF17 AA2:AA17</xm:sqref>
+          <xm:sqref>W13:W16 AA2:AA16 AF2:AF16 W2:W9 V2:V16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{03EA1083-D949-46E8-A92C-28C1E75A14F4}">
           <x14:formula1>
             <xm:f>Tables!$G$2:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AD2:AD17 Y2:Y17</xm:sqref>
+          <xm:sqref>Y2:Y16 AD2:AD16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{296B0321-4EB3-4DBF-B3C7-556564F8D22F}">
           <x14:formula1>
             <xm:f>Tables!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>Z2:Z17 AE2:AE17</xm:sqref>
+          <xm:sqref>AE2:AE16 Z2:Z16</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{4E0921CE-AE87-4561-B95D-97362BD64B5C}">
           <x14:formula1>
-            <xm:f>Tables!$I$2:$I$42</xm:f>
+            <xm:f>Tables!$I$2:$I$45</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D17</xm:sqref>
+          <xm:sqref>D2:D16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2321,12 +2274,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
       <c r="E1" s="32"/>
       <c r="F1" s="32"/>
       <c r="G1" s="31"/>
@@ -2347,12 +2300,12 @@
       <c r="D2" s="26"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
@@ -2393,19 +2346,19 @@
       <c r="D8" s="13"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="51"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
@@ -2491,55 +2444,55 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="50" t="s">
+      <c r="A15" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="46"/>
-      <c r="H15" s="46"/>
-      <c r="I15" s="46"/>
-      <c r="J15" s="47"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="49"/>
       <c r="K15" s="28">
         <f>SUM(K12:K14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="52" t="s">
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="54" t="s">
         <v>68</v>
       </c>
-      <c r="I16" s="52"/>
-      <c r="J16" s="53"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="55"/>
       <c r="K16" s="29">
         <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="47"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="49"/>
       <c r="K17" s="27">
         <f>SUM(K15:K16)</f>
         <v>150</v>
@@ -2576,10 +2529,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="55"/>
+      <c r="B1" s="57"/>
       <c r="C1" s="30"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2629,10 +2582,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7C7130-C7ED-4E34-8ED2-CC717737ADA7}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I42" sqref="I1:I42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2654,10 +2607,10 @@
         <v>37</v>
       </c>
       <c r="G1" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="I1" s="56" t="s">
-        <v>151</v>
+        <v>93</v>
+      </c>
+      <c r="I1" s="43" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2665,7 +2618,7 @@
       <c r="C2" s="11"/>
       <c r="E2" s="11"/>
       <c r="G2" s="11"/>
-      <c r="I2" s="11"/>
+      <c r="I2" s="44"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -2678,10 +2631,10 @@
         <v>6</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="I3" s="57" t="s">
-        <v>119</v>
+        <v>94</v>
+      </c>
+      <c r="I3" s="44" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2695,10 +2648,10 @@
         <v>43</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="I4" s="57" t="s">
-        <v>120</v>
+        <v>95</v>
+      </c>
+      <c r="I4" s="44" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2712,10 +2665,10 @@
         <v>8</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="I5" s="57" t="s">
-        <v>121</v>
+        <v>96</v>
+      </c>
+      <c r="I5" s="44" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2729,10 +2682,10 @@
         <v>44</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="I6" s="57" t="s">
-        <v>122</v>
+        <v>97</v>
+      </c>
+      <c r="I6" s="44" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2742,8 +2695,8 @@
       <c r="E7" s="11">
         <v>9</v>
       </c>
-      <c r="I7" s="57" t="s">
-        <v>123</v>
+      <c r="I7" s="44" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2753,7 +2706,7 @@
       <c r="E8" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="57" t="s">
+      <c r="I8" s="44" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2764,7 +2717,7 @@
       <c r="E9" s="11">
         <v>10</v>
       </c>
-      <c r="I9" s="57" t="s">
+      <c r="I9" s="44" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2775,8 +2728,8 @@
       <c r="E10" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="57" t="s">
-        <v>124</v>
+      <c r="I10" s="44" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2786,8 +2739,8 @@
       <c r="E11" s="11">
         <v>11</v>
       </c>
-      <c r="I11" s="57" t="s">
-        <v>125</v>
+      <c r="I11" s="44" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2797,8 +2750,8 @@
       <c r="E12" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="57" t="s">
-        <v>126</v>
+      <c r="I12" s="44" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2806,165 +2759,183 @@
       <c r="E13" s="11">
         <v>12</v>
       </c>
-      <c r="I13" s="57" t="s">
-        <v>18</v>
+      <c r="I13" s="44" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E14" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="I14" s="57" t="s">
-        <v>127</v>
+      <c r="I14" s="44" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E15" s="11">
         <v>14</v>
       </c>
-      <c r="I15" s="57" t="s">
-        <v>128</v>
+      <c r="I15" s="44" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="I16" s="57" t="s">
+      <c r="I16" s="44" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I17" s="44" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="44" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I19" s="44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I20" s="44" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="44" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I22" s="44" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I17" s="57" t="s">
+    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="44" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I18" s="57" t="s">
+    <row r="24" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I24" s="44" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I25" s="44" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I19" s="57" t="s">
+    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I26" s="44" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I20" s="57" t="s">
+    <row r="27" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I27" s="44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I28" s="44" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I21" s="57" t="s">
+    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I29" s="44" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I22" s="57" t="s">
+    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I30" s="44" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I23" s="57" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I24" s="57" t="s">
+    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I31" s="44" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I25" s="57" t="s">
+    <row r="32" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I32" s="44" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I33" s="44" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I34" s="44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="44" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I26" s="57" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I27" s="57" t="s">
+    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I36" s="44" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I28" s="57" t="s">
+    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I37" s="44" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I29" s="57" t="s">
+    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I38" s="44" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I30" s="57" t="s">
+    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I39" s="44" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I31" s="57" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I32" s="57" t="s">
+    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I40" s="44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I41" s="44" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I33" s="57" t="s">
+    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I42" s="44" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I34" s="57" t="s">
+    <row r="43" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I43" s="44" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I35" s="57" t="s">
+    <row r="44" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I44" s="44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I45" s="44" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I36" s="57" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I37" s="57" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I38" s="57" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I39" s="57" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I40" s="57" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I41" s="57" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I42" s="57" t="s">
-        <v>150</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I3:I45">
+    <sortCondition ref="I3:I45"/>
+  </sortState>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:F2 O2:XFD2" xr:uid="{C5F5580C-CDE8-4810-9011-46F88A3A0968}">
       <formula1>$A$4:$A$10</formula1>

</xml_diff>

<commit_message>
Added the line weight when selecting a Dotted connection pattern. Fixed a bug when selecting Dash line pattern
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_BlueprintingDataFile_Template.xlsx
+++ b/Data/ScriptData/OC_BlueprintingDataFile_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Blueprinting_Tool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BFF9A0-DF70-4695-8F60-A4EAA4C137D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E385127-0288-4356-BA93-E50888696F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20310" yWindow="1635" windowWidth="26505" windowHeight="15330" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
+    <workbookView xWindow="25605" yWindow="750" windowWidth="26505" windowHeight="15330" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -235,7 +235,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="153">
   <si>
     <t>mach_name</t>
   </si>
@@ -549,14 +549,8 @@
     <t>xxx.xxx.xxx.xxx</t>
   </si>
   <si>
-    <t>Server:OSI-T1</t>
-  </si>
-  <si>
     <t>OIS Test Server
 Cloud Hosted</t>
-  </si>
-  <si>
-    <t>OISInterfaces:T1</t>
   </si>
   <si>
     <t>OISInterfaces</t>
@@ -1348,9 +1342,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AF16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1566,7 +1560,7 @@
         <v>79</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D4" s="38"/>
       <c r="E4" s="38" t="s">
@@ -1652,7 +1646,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>15</v>
@@ -1702,7 +1696,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>17</v>
@@ -1754,7 +1748,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>18</v>
@@ -1844,7 +1838,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>99</v>
@@ -1887,7 +1881,7 @@
       <c r="Z10" s="11"/>
       <c r="AA10" s="7"/>
       <c r="AB10" s="8" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="AC10" s="7"/>
       <c r="AD10" s="11" t="s">
@@ -1908,13 +1902,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>99</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
@@ -1951,7 +1945,7 @@
       <c r="Z11" s="11"/>
       <c r="AA11" s="7"/>
       <c r="AB11" s="8" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="AC11" s="7"/>
       <c r="AD11" s="11" t="s">
@@ -1972,13 +1966,13 @@
         <v>14</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
@@ -2022,13 +2016,13 @@
     </row>
     <row r="13" spans="1:32" s="6" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
@@ -2066,7 +2060,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>15</v>
@@ -2116,7 +2110,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>17</v>
@@ -2168,7 +2162,7 @@
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>18</v>
@@ -2610,7 +2604,7 @@
         <v>93</v>
       </c>
       <c r="I1" s="43" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2634,7 +2628,7 @@
         <v>94</v>
       </c>
       <c r="I3" s="44" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2651,7 +2645,7 @@
         <v>95</v>
       </c>
       <c r="I4" s="44" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2668,7 +2662,7 @@
         <v>96</v>
       </c>
       <c r="I5" s="44" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2685,7 +2679,7 @@
         <v>97</v>
       </c>
       <c r="I6" s="44" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2696,7 +2690,7 @@
         <v>9</v>
       </c>
       <c r="I7" s="44" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2729,7 +2723,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="44" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2740,7 +2734,7 @@
         <v>11</v>
       </c>
       <c r="I11" s="44" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2751,7 +2745,7 @@
         <v>47</v>
       </c>
       <c r="I12" s="44" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2760,7 +2754,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="44" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2776,7 +2770,7 @@
         <v>14</v>
       </c>
       <c r="I15" s="44" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2784,42 +2778,42 @@
         <v>49</v>
       </c>
       <c r="I16" s="44" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I17" s="44" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I18" s="44" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I19" s="44" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I20" s="44" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I21" s="44" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I22" s="44" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I23" s="44" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="9:9" x14ac:dyDescent="0.25">
@@ -2829,37 +2823,37 @@
     </row>
     <row r="25" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I25" s="44" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I26" s="44" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I27" s="44" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I28" s="44" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I29" s="44" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I30" s="44" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I31" s="44" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="9:9" x14ac:dyDescent="0.25">
@@ -2869,37 +2863,37 @@
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I33" s="44" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I34" s="44" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I35" s="44" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I36" s="44" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="37" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I37" s="44" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I38" s="44" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I39" s="44" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="9:9" x14ac:dyDescent="0.25">
@@ -2909,17 +2903,17 @@
     </row>
     <row r="41" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I41" s="44" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I42" s="44" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I43" s="44" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="44" spans="9:9" x14ac:dyDescent="0.25">
@@ -2929,7 +2923,7 @@
     </row>
     <row r="45" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I45" s="44" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new stencils.   Update the user guide.   updated the excel data templates
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_BlueprintingDataFile_Template.xlsx
+++ b/Data/ScriptData/OC_BlueprintingDataFile_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell\Workspace\winApps\OmnicellBlueprintingTool\Data\ScriptData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Blueprinting_Tool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5809D90F-59DE-42BE-A97B-84B9C8C72A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CBFE02-A592-45BE-A630-A0A3CD5F54A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27300" yWindow="345" windowWidth="26505" windowHeight="14415" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
+    <workbookView xWindow="2265" yWindow="690" windowWidth="23910" windowHeight="14415" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -644,16 +644,7 @@
     <t>PortsLDAP_info</t>
   </si>
   <si>
-    <t>Process1</t>
-  </si>
-  <si>
-    <t>Rectangle</t>
-  </si>
-  <si>
     <t>Site</t>
-  </si>
-  <si>
-    <t>Square</t>
   </si>
   <si>
     <t>Supply</t>
@@ -700,9 +691,6 @@
   </si>
   <si>
     <t>Group4</t>
-  </si>
-  <si>
-    <t>C:\Omnicell_Blueprinting_Tool\Data\Stencils\Account_CustomStencils.vssx</t>
   </si>
   <si>
     <t>Page Setup</t>
@@ -766,6 +754,18 @@
       </rPr>
       <t xml:space="preserve"> (default), Tabloid, Ledger, Legal, A3, A4</t>
     </r>
+  </si>
+  <si>
+    <t>OC-Process</t>
+  </si>
+  <si>
+    <t>OC-Rectangle</t>
+  </si>
+  <si>
+    <t>OC-Square</t>
+  </si>
+  <si>
+    <t>C:\Omnicell_Blueprinting_Tool\Data\Stencils\OC_BlueprintingStencils.vssx</t>
   </si>
 </sst>
 </file>
@@ -1078,7 +1078,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1421,7 +1421,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,8 +1580,8 @@
       <c r="AF2" s="16"/>
     </row>
     <row r="3" spans="1:32" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="37">
-        <v>0</v>
+      <c r="A3" s="37" t="s">
+        <v>78</v>
       </c>
       <c r="B3" s="38" t="s">
         <v>77</v>
@@ -1630,14 +1630,14 @@
       <c r="AF3" s="7"/>
     </row>
     <row r="4" spans="1:32" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
-        <v>78</v>
+      <c r="A4" s="37">
+        <v>0</v>
       </c>
       <c r="B4" s="38" t="s">
         <v>79</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="D4" s="38"/>
       <c r="E4" s="38" t="s">
@@ -1684,14 +1684,14 @@
         <v>78</v>
       </c>
       <c r="B5" s="38" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="D5" s="38"/>
       <c r="E5" s="38" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
@@ -2143,13 +2143,13 @@
     </row>
     <row r="14" spans="1:32" s="6" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
@@ -2731,7 +2731,7 @@
         <v>93</v>
       </c>
       <c r="I1" s="43" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2850,7 +2850,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="45" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2861,7 +2861,7 @@
         <v>11</v>
       </c>
       <c r="I11" s="44" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2897,7 +2897,7 @@
         <v>14</v>
       </c>
       <c r="I15" s="44" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2905,7 +2905,7 @@
         <v>49</v>
       </c>
       <c r="I16" s="45" t="s">
-        <v>157</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.25">
@@ -2920,12 +2920,12 @@
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I19" s="44" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I20" s="44" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.25">
@@ -2970,72 +2970,72 @@
     </row>
     <row r="29" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I29" s="45" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I30" s="44" t="s">
-        <v>103</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I31" s="44" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I32" s="44" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I33" s="44" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I34" s="44" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I35" s="44" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I36" s="44" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I37" s="44" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I38" s="44" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I39" s="44" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I40" s="44" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I41" s="44" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I42" s="44" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="9:9" x14ac:dyDescent="0.25">
@@ -3045,17 +3045,17 @@
     </row>
     <row r="44" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I44" s="44" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I45" s="44" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I46" s="44" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="9:9" x14ac:dyDescent="0.25">
@@ -3065,7 +3065,7 @@
     </row>
     <row r="48" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I48" s="44" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifications to the blueprinting template excel files
</commit_message>
<xml_diff>
--- a/Data/ScriptData/OC_BlueprintingDataFile_Template.xlsx
+++ b/Data/ScriptData/OC_BlueprintingDataFile_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Omnicell_Blueprinting_Tool\Data\ScriptData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1E8920-56FE-46CA-90D6-D8616AB5E077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFAAD2D-1BEF-4A7F-9BD9-84681F623F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25275" yWindow="570" windowWidth="22200" windowHeight="14415" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
+    <workbookView xWindow="2025" yWindow="2310" windowWidth="22200" windowHeight="14415" xr2:uid="{F7C08203-2112-4032-A78B-91DB85A7B88A}"/>
   </bookViews>
   <sheets>
     <sheet name="VisioData" sheetId="1" r:id="rId1"/>
@@ -235,7 +235,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="166">
   <si>
     <t>mach_name</t>
   </si>
@@ -470,12 +470,6 @@
   </si>
   <si>
     <t>;Visio Section</t>
-  </si>
-  <si>
-    <t>Using a Visio Template that contains a custom Stencil</t>
-  </si>
-  <si>
-    <t>Custom Stencil</t>
   </si>
   <si>
     <t>C:\Omnicell_Blueprinting_Tool\Data\Templates\OC_BlueprintingTemplate.vstx</t>
@@ -781,6 +775,20 @@
   </si>
   <si>
     <t>OC_Square2</t>
+  </si>
+  <si>
+    <t>Autosize:true</t>
+  </si>
+  <si>
+    <t>• true - Autosize all pages
+• false - (default) don't Autosize the pages</t>
+  </si>
+  <si>
+    <t>Use the Blueprinting Visio Template.  Already contains the OC_BlueprintingStencils.vssx stencil</t>
+  </si>
+  <si>
+    <t>Custom Stencil - Add this stencil OC_BlueprintingStencils to the Visio Diagram
+Create a row for each custom stencil to add to the document</t>
   </si>
 </sst>
 </file>
@@ -973,7 +981,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1095,6 +1103,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1432,11 +1443,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6B3580-88F6-4152-BCD8-7BDA3AA42961}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AF17"/>
+  <dimension ref="A1:AF18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,7 +1479,7 @@
         <v>35</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D1" s="40" t="s">
         <v>36</v>
@@ -1477,7 +1488,7 @@
         <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
@@ -1531,31 +1542,31 @@
         <v>30</v>
       </c>
       <c r="X1" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z1" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="Y1" s="18" t="s">
+      <c r="AA1" s="18" t="s">
         <v>82</v>
-      </c>
-      <c r="Z1" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA1" s="18" t="s">
-        <v>84</v>
       </c>
       <c r="AB1" s="5" t="s">
         <v>33</v>
       </c>
       <c r="AC1" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD1" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE1" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="AD1" s="19" t="s">
+      <c r="AF1" s="19" t="s">
         <v>86</v>
-      </c>
-      <c r="AE1" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF1" s="19" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -1602,11 +1613,11 @@
         <v>73</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8" t="s">
-        <v>77</v>
+        <v>164</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -1644,7 +1655,7 @@
       <c r="AE3" s="11"/>
       <c r="AF3" s="7"/>
     </row>
-    <row r="4" spans="1:32" s="12" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" s="12" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="36">
         <v>0</v>
       </c>
@@ -1652,11 +1663,11 @@
         <v>75</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D4" s="37"/>
       <c r="E4" s="37" t="s">
-        <v>78</v>
+        <v>165</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
@@ -1699,14 +1710,14 @@
         <v>74</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D5" s="37"/>
       <c r="E5" s="37" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
@@ -1744,93 +1755,93 @@
       <c r="AE5" s="11"/>
       <c r="AF5" s="7"/>
     </row>
-    <row r="6" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:32" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>0</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46" t="s">
+        <v>163</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="10">
+        <v>0</v>
+      </c>
+      <c r="S6" s="10">
+        <v>0</v>
+      </c>
+      <c r="T6" s="10">
+        <v>0</v>
+      </c>
+      <c r="U6" s="10">
+        <v>0</v>
+      </c>
+      <c r="V6" s="10"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="7"/>
+    </row>
+    <row r="7" spans="1:32" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="15"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="17"/>
-      <c r="W6" s="14"/>
-      <c r="X6" s="16"/>
-      <c r="Y6" s="16"/>
-      <c r="Z6" s="16"/>
-      <c r="AA6" s="16"/>
-      <c r="AB6" s="16"/>
-      <c r="AC6" s="16"/>
-      <c r="AD6" s="16"/>
-      <c r="AE6" s="16"/>
-      <c r="AF6" s="16"/>
-    </row>
-    <row r="7" spans="1:32" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
-        <v>1</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="S7" s="10">
-        <v>10.75</v>
-      </c>
-      <c r="T7" s="10">
-        <v>0</v>
-      </c>
-      <c r="U7" s="10">
-        <v>0</v>
-      </c>
-      <c r="V7" s="10"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="7"/>
-      <c r="AC7" s="7"/>
-      <c r="AD7" s="11"/>
-      <c r="AE7" s="11"/>
-      <c r="AF7" s="7"/>
-    </row>
-    <row r="8" spans="1:32" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="16"/>
+      <c r="AC7" s="16"/>
+      <c r="AD7" s="16"/>
+      <c r="AE7" s="16"/>
+      <c r="AF7" s="16"/>
+    </row>
+    <row r="8" spans="1:32" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>1</v>
       </c>
@@ -1838,14 +1849,12 @@
         <v>14</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>28</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="E8" s="21"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -1859,7 +1868,7 @@
       <c r="P8" s="9"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="10">
-        <v>3.125</v>
+        <v>0.25</v>
       </c>
       <c r="S8" s="10">
         <v>10.75</v>
@@ -1882,7 +1891,7 @@
       <c r="AE8" s="11"/>
       <c r="AF8" s="7"/>
     </row>
-    <row r="9" spans="1:32" s="12" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>1</v>
       </c>
@@ -1890,17 +1899,15 @@
         <v>14</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="8">
-        <v>10</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -1911,18 +1918,18 @@
       <c r="N9" s="8"/>
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="S9" s="9">
-        <v>1.75</v>
-      </c>
-      <c r="T9" s="9">
-        <v>0</v>
-      </c>
-      <c r="U9" s="9">
-        <v>1.125</v>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="10">
+        <v>3.125</v>
+      </c>
+      <c r="S9" s="10">
+        <v>10.75</v>
+      </c>
+      <c r="T9" s="10">
+        <v>0</v>
+      </c>
+      <c r="U9" s="10">
+        <v>0</v>
       </c>
       <c r="V9" s="10"/>
       <c r="W9" s="8"/>
@@ -1936,107 +1943,97 @@
       <c r="AE9" s="11"/>
       <c r="AF9" s="7"/>
     </row>
-    <row r="10" spans="1:32" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="17"/>
-      <c r="S10" s="17"/>
-      <c r="T10" s="17"/>
-      <c r="U10" s="17"/>
-      <c r="V10" s="17"/>
-      <c r="W10" s="14"/>
-      <c r="X10" s="16"/>
-      <c r="Y10" s="16"/>
-      <c r="Z10" s="16"/>
-      <c r="AA10" s="16"/>
-      <c r="AB10" s="16"/>
-      <c r="AC10" s="16"/>
-      <c r="AD10" s="16"/>
-      <c r="AE10" s="16"/>
-      <c r="AF10" s="16"/>
-    </row>
-    <row r="11" spans="1:32" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+    <row r="10" spans="1:32" s="12" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
         <v>1</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="10">
-        <v>4.875</v>
-      </c>
-      <c r="S11" s="10">
-        <v>6.25</v>
-      </c>
-      <c r="T11" s="10">
-        <v>0</v>
-      </c>
-      <c r="U11" s="10">
-        <v>0</v>
-      </c>
-      <c r="V11" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="W11" s="8"/>
-      <c r="X11" s="7"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="11"/>
-      <c r="AA11" s="7"/>
-      <c r="AB11" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="AC11" s="7"/>
-      <c r="AD11" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE11" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="AF11" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C10" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="8">
+        <v>10</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="S10" s="9">
+        <v>1.75</v>
+      </c>
+      <c r="T10" s="9">
+        <v>0</v>
+      </c>
+      <c r="U10" s="9">
+        <v>1.125</v>
+      </c>
+      <c r="V10" s="10"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="7"/>
+    </row>
+    <row r="11" spans="1:32" s="6" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="16"/>
+      <c r="AB11" s="16"/>
+      <c r="AC11" s="16"/>
+      <c r="AD11" s="16"/>
+      <c r="AE11" s="16"/>
+      <c r="AF11" s="16"/>
+    </row>
+    <row r="12" spans="1:32" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>1</v>
       </c>
@@ -2044,13 +2041,13 @@
         <v>14</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
@@ -2062,15 +2059,15 @@
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
       <c r="O12" s="9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="P12" s="9"/>
       <c r="Q12" s="7"/>
       <c r="R12" s="10">
-        <v>6.125</v>
+        <v>4.875</v>
       </c>
       <c r="S12" s="10">
-        <v>5.7969999999999997</v>
+        <v>6.25</v>
       </c>
       <c r="T12" s="10">
         <v>0</v>
@@ -2087,14 +2084,14 @@
       <c r="Z12" s="11"/>
       <c r="AA12" s="7"/>
       <c r="AB12" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="AC12" s="7"/>
       <c r="AD12" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="AE12" s="11" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="AF12" s="7" t="s">
         <v>17</v>
@@ -2108,13 +2105,13 @@
         <v>14</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -2126,17 +2123,15 @@
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
       <c r="O13" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="P13" s="9">
-        <v>5001</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="P13" s="9"/>
       <c r="Q13" s="7"/>
       <c r="R13" s="10">
-        <v>7.5</v>
+        <v>6.125</v>
       </c>
       <c r="S13" s="10">
-        <v>6.0750000000000002</v>
+        <v>5.7969999999999997</v>
       </c>
       <c r="T13" s="10">
         <v>0</v>
@@ -2144,107 +2139,123 @@
       <c r="U13" s="10">
         <v>0</v>
       </c>
-      <c r="V13" s="10"/>
+      <c r="V13" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="W13" s="8"/>
       <c r="X13" s="7"/>
       <c r="Y13" s="11"/>
       <c r="Z13" s="11"/>
       <c r="AA13" s="7"/>
-      <c r="AB13" s="7"/>
+      <c r="AB13" s="8" t="s">
+        <v>102</v>
+      </c>
       <c r="AC13" s="7"/>
-      <c r="AD13" s="11"/>
-      <c r="AE13" s="11"/>
-      <c r="AF13" s="7"/>
-    </row>
-    <row r="14" spans="1:32" s="6" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="17"/>
-      <c r="S14" s="17"/>
-      <c r="T14" s="17"/>
-      <c r="U14" s="17"/>
-      <c r="V14" s="17"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="16"/>
-      <c r="Y14" s="16"/>
-      <c r="Z14" s="16"/>
-      <c r="AA14" s="16"/>
-      <c r="AB14" s="16"/>
-      <c r="AC14" s="16"/>
-      <c r="AD14" s="16"/>
-      <c r="AE14" s="16"/>
-      <c r="AF14" s="16"/>
-    </row>
-    <row r="15" spans="1:32" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
-        <v>2</v>
-      </c>
-      <c r="B15" s="8" t="s">
+      <c r="AD13" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE13" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF13" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>1</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="E15" s="21"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="10">
-        <v>0.25</v>
-      </c>
-      <c r="S15" s="10">
-        <v>10.75</v>
-      </c>
-      <c r="T15" s="10">
-        <v>0</v>
-      </c>
-      <c r="U15" s="10">
-        <v>0</v>
-      </c>
-      <c r="V15" s="10"/>
-      <c r="W15" s="8"/>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="7"/>
-      <c r="AB15" s="7"/>
-      <c r="AC15" s="7"/>
-      <c r="AD15" s="11"/>
-      <c r="AE15" s="11"/>
-      <c r="AF15" s="7"/>
-    </row>
-    <row r="16" spans="1:32" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="C14" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="P14" s="9">
+        <v>5001</v>
+      </c>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="10">
+        <v>7.5</v>
+      </c>
+      <c r="S14" s="10">
+        <v>6.0750000000000002</v>
+      </c>
+      <c r="T14" s="10">
+        <v>0</v>
+      </c>
+      <c r="U14" s="10">
+        <v>0</v>
+      </c>
+      <c r="V14" s="10"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="11"/>
+      <c r="AF14" s="7"/>
+    </row>
+    <row r="15" spans="1:32" s="6" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="16"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="16"/>
+      <c r="Z15" s="16"/>
+      <c r="AA15" s="16"/>
+      <c r="AB15" s="16"/>
+      <c r="AC15" s="16"/>
+      <c r="AD15" s="16"/>
+      <c r="AE15" s="16"/>
+      <c r="AF15" s="16"/>
+    </row>
+    <row r="16" spans="1:32" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>2</v>
       </c>
@@ -2252,14 +2263,12 @@
         <v>14</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>28</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="E16" s="21"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -2273,7 +2282,7 @@
       <c r="P16" s="9"/>
       <c r="Q16" s="7"/>
       <c r="R16" s="10">
-        <v>3.125</v>
+        <v>0.25</v>
       </c>
       <c r="S16" s="10">
         <v>10.75</v>
@@ -2296,7 +2305,7 @@
       <c r="AE16" s="11"/>
       <c r="AF16" s="7"/>
     </row>
-    <row r="17" spans="1:32" s="12" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" s="12" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>2</v>
       </c>
@@ -2304,17 +2313,15 @@
         <v>14</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="8">
-        <v>10</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
@@ -2325,18 +2332,18 @@
       <c r="N17" s="8"/>
       <c r="O17" s="9"/>
       <c r="P17" s="9"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="S17" s="9">
-        <v>1.75</v>
-      </c>
-      <c r="T17" s="9">
-        <v>0</v>
-      </c>
-      <c r="U17" s="9">
-        <v>1.125</v>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="10">
+        <v>3.125</v>
+      </c>
+      <c r="S17" s="10">
+        <v>10.75</v>
+      </c>
+      <c r="T17" s="10">
+        <v>0</v>
+      </c>
+      <c r="U17" s="10">
+        <v>0</v>
       </c>
       <c r="V17" s="10"/>
       <c r="W17" s="8"/>
@@ -2350,6 +2357,60 @@
       <c r="AE17" s="11"/>
       <c r="AF17" s="7"/>
     </row>
+    <row r="18" spans="1:32" s="12" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>2</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="8">
+        <v>10</v>
+      </c>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="S18" s="9">
+        <v>1.75</v>
+      </c>
+      <c r="T18" s="9">
+        <v>0</v>
+      </c>
+      <c r="U18" s="9">
+        <v>1.125</v>
+      </c>
+      <c r="V18" s="10"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="11"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="11"/>
+      <c r="AF18" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2361,25 +2422,25 @@
           <x14:formula1>
             <xm:f>Tables!$E$2:$E$16</xm:f>
           </x14:formula1>
-          <xm:sqref>F7:F10 F14:F17</xm:sqref>
+          <xm:sqref>F8:F11 F15:F18</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{E07EFBB9-D469-4A17-B52C-CFA259DBA49F}">
           <x14:formula1>
             <xm:f>Tables!$A$2:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>W14:W17 W5:W10 V5:V17 V2:W4 AF2:AF17 AA2:AA17</xm:sqref>
+          <xm:sqref>W15:W18 V7:V18 AF7:AF18 AA7:AA18 AF2:AF5 V2:W5 W7:W11 AA2:AA5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{03EA1083-D949-46E8-A92C-28C1E75A14F4}">
           <x14:formula1>
             <xm:f>Tables!$G$2:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>AD2:AD17 Y2:Y17</xm:sqref>
+          <xm:sqref>Y7:Y18 AD2:AD5 AD7:AD18 Y2:Y5</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{296B0321-4EB3-4DBF-B3C7-556564F8D22F}">
           <x14:formula1>
             <xm:f>Tables!$C$2:$C$6</xm:f>
           </x14:formula1>
-          <xm:sqref>Z2:Z17 AE2:AE17</xm:sqref>
+          <xm:sqref>AE7:AE18 Z2:Z5 Z7:Z18 AE2:AE5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2404,12 +2465,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="31"/>
       <c r="F1" s="31"/>
       <c r="G1" s="30"/>
@@ -2430,12 +2491,12 @@
       <c r="D2" s="25"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
@@ -2476,19 +2537,19 @@
       <c r="D8" s="13"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="52"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
@@ -2574,55 +2635,55 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="B15" s="49"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="50"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="51"/>
       <c r="K15" s="27">
         <f>SUM(K12:K14)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="55" t="s">
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="I16" s="55"/>
-      <c r="J16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="57"/>
       <c r="K16" s="28">
         <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="49"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="50"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="51"/>
       <c r="K17" s="26">
         <f>SUM(K15:K16)</f>
         <v>150</v>
@@ -2659,10 +2720,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="58"/>
+      <c r="B1" s="59"/>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2737,10 +2798,10 @@
         <v>34</v>
       </c>
       <c r="G1" s="38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2761,10 +2822,10 @@
         <v>6</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I3" s="43" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2778,10 +2839,10 @@
         <v>39</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I4" s="43" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2795,10 +2856,10 @@
         <v>8</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I5" s="43" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2812,10 +2873,10 @@
         <v>40</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I6" s="43" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2826,7 +2887,7 @@
         <v>9</v>
       </c>
       <c r="I7" s="43" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2837,7 +2898,7 @@
         <v>41</v>
       </c>
       <c r="I8" s="43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2848,7 +2909,7 @@
         <v>10</v>
       </c>
       <c r="I9" s="43" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2859,7 +2920,7 @@
         <v>42</v>
       </c>
       <c r="I10" s="44" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2870,7 +2931,7 @@
         <v>11</v>
       </c>
       <c r="I11" s="43" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2881,7 +2942,7 @@
         <v>43</v>
       </c>
       <c r="I12" s="43" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2890,7 +2951,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="43" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2898,7 +2959,7 @@
         <v>44</v>
       </c>
       <c r="I14" s="43" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2906,7 +2967,7 @@
         <v>14</v>
       </c>
       <c r="I15" s="43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2914,177 +2975,177 @@
         <v>45</v>
       </c>
       <c r="I16" s="44" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I17" s="43" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I18" s="43" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I19" s="43" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I20" s="43" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I21" s="43" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I22" s="43" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I23" s="43" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I24" s="43" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I25" s="43" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I26" s="43" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I27" s="43" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I28" s="43" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I29" s="44" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I30" s="43" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I31" s="43" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I32" s="45" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I33" s="43" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I34" s="43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I35" s="43" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I36" s="43" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I37" s="43" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I38" s="43" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I39" s="43" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I40" s="43" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I41" s="43" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I42" s="43" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="43" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I43" s="43" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I44" s="43" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I45" s="43" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I46" s="43" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I47" s="43" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="48" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I48" s="43" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I49" s="43" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="50" spans="9:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I50" s="43" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>